<commit_message>
Mappa di traduzione aggiornata
</commit_message>
<xml_diff>
--- a/mappeNuove.xlsx
+++ b/mappeNuove.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\UninaCampus\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="89">
   <si>
     <t>Azione</t>
   </si>
@@ -432,9 +432,6 @@
     <t>solo.clickOnView(solo.getView(R.id.idspinner));</t>
   </si>
   <si>
-    <t>Spinner s = solo.getView(R.id.idspinner); solo.clickOnView(s.getChildAt(4))</t>
-  </si>
-  <si>
     <t>solo.clickLongOnView(solo.getView(R.id.idBottone));</t>
   </si>
   <si>
@@ -444,10 +441,14 @@
     <t>Spinner s = (Spinner)solo.getView(R.id.idSPinner); assertEquals("Ingegneria", s.getSelectedItem().toString());</t>
   </si>
   <si>
-    <t>ListView lv = solo.getView(R.id.listaSceltaCorsi); assertEquals("universita", lv.getSelectedItem().toString());</t>
-  </si>
-  <si>
-    <t>((TextView)solo.getView(R.id.idText)).setText("ciao!");</t>
+    <t>Spinner s = (Spinner)solo.getView(R.id.idspinner);
+        solo.clickOnView(s);
+        solo.scrollToTop(); // I put this in here so that it always keeps the list at start
+        // select the 3th item in the spinner
+        solo.clickOnView(solo.getView(TextView.class, 3));</t>
+  </si>
+  <si>
+    <t>solo.enterText((EditText) solo.getView(R.id.idtextView), "idinputText!");</t>
   </si>
 </sst>
 </file>
@@ -895,15 +896,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43.7109375" customWidth="1"/>
     <col min="2" max="2" width="62.140625" customWidth="1"/>
-    <col min="3" max="3" width="50" customWidth="1"/>
+    <col min="3" max="3" width="74.140625" customWidth="1"/>
     <col min="4" max="4" width="139.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -984,8 +985,8 @@
       <c r="B6" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D6" t="s">
-        <v>84</v>
+      <c r="D6" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="135" x14ac:dyDescent="0.25">
@@ -1026,6 +1027,9 @@
       <c r="C9" t="s">
         <v>19</v>
       </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="10" spans="1:4" ht="152.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -1038,7 +1042,7 @@
         <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="200.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1052,7 +1056,7 @@
         <v>67</v>
       </c>
       <c r="D11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="226.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1150,7 +1154,7 @@
         <v>73</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1164,7 +1168,7 @@
         <v>40</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>88</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="181.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1191,6 +1195,9 @@
       <c r="C21" t="s">
         <v>44</v>
       </c>
+      <c r="D21" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="22" spans="1:4" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
@@ -1202,6 +1209,9 @@
       <c r="C22" t="s">
         <v>46</v>
       </c>
+      <c r="D22" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="23" spans="1:4" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
@@ -1214,7 +1224,7 @@
         <v>48</v>
       </c>
       <c r="D23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="164.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Inserimento progetto VPP e aggiornamento delle Mappe
</commit_message>
<xml_diff>
--- a/mappeNuove.xlsx
+++ b/mappeNuove.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\UninaCampus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikel_000\Desktop\ProgettoIS2\UninaCampus\UninaCampus\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="91">
   <si>
     <t>Azione</t>
   </si>
@@ -273,28 +273,6 @@
         linearLayout.perform(click());</t>
   </si>
   <si>
-    <t xml:space="preserve">        DataInteraction appCompatTextView52 = onData(anything())
-                .inAdapterView(allOf(withId(R.id.idLista),
-                        childAtPosition(
-                                withClassName(is("android.widget.LinearLayout")),
-                                6)))
-                .atPosition(3);
-        appCompatTextView52.perform(longClick());
-                                       </t>
-  </si>
-  <si>
-    <t xml:space="preserve">        ViewInteraction appCompatButton0 = onView(
-                allOf(withId(R.id.dialogoButton), withText("Apri Dialog"),
-                        childAtPosition(
-                                childAtPosition(
-                                        withClassName(is("android.support.constraint.ConstraintLayout")),
-                                        0),
-                                4),
-                        isDisplayed()));
-        appCompatButton0.perform(longClick());
-        </t>
-  </si>
-  <si>
     <t xml:space="preserve">        ListView lista= (ListView) activity.findViewById(R.id.idLista);
         assertTrue(lista.isLongClickable());
         AdapterView.OnItemLongClickListener iteml=lista.getOnItemLongClickListener();
@@ -449,6 +427,34 @@
   </si>
   <si>
     <t>solo.enterText((EditText) solo.getView(R.id.idtextView), "idinputText!");</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ((Spinner) activity.findViewById(R.id.idspinner)).setSelection(1);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         DataInteraction appCompatTextView52 = onData(anything())
+                .inAdapterView(allOf(withId(R.id.idLista),
+                        childAtPosition(
+                                withClassName(is("android.widget.LinearLayout")),
+                                6)))
+                .atPosition(3);
+        appCompatTextView52.perform(longClick());
+        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        ViewInteraction appCompatButton0 = onView(
+                allOf(withId(R.id.dialogoButton), withText("Apri Dialog"),
+                        childAtPosition(
+                                childAtPosition(
+                                        withClassName(is("android.support.constraint.ConstraintLayout")),
+                                        0),
+                                4),
+                        isDisplayed()));
+        appCompatButton0.perform(longClick());
+                                       </t>
+  </si>
+  <si>
+    <t>solo.waitForActivity(Activity.class, 500); (verifica la nuova activity)  oppure solo.assertCurrentActivity("Nope", Activity.class);</t>
   </si>
 </sst>
 </file>
@@ -896,8 +902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,7 +953,7 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="189.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -961,7 +967,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="156.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -975,7 +981,7 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="156.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -985,11 +991,14 @@
       <c r="B6" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="C6" t="s">
+        <v>87</v>
+      </c>
       <c r="D6" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="165" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
@@ -1000,7 +1009,7 @@
         <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="195" customHeight="1" x14ac:dyDescent="0.25">
@@ -1031,32 +1040,32 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="152.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="234" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="200.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="212.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="226.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1064,7 +1073,7 @@
         <v>23</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C12" t="s">
         <v>24</v>
@@ -1078,7 +1087,7 @@
         <v>25</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C13" t="s">
         <v>26</v>
@@ -1092,7 +1101,7 @@
         <v>27</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C14" t="s">
         <v>28</v>
@@ -1106,7 +1115,7 @@
         <v>29</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C15" t="s">
         <v>30</v>
@@ -1120,7 +1129,7 @@
         <v>31</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C16" t="s">
         <v>32</v>
@@ -1148,13 +1157,13 @@
         <v>37</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1176,13 +1185,13 @@
         <v>41</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C20" t="s">
         <v>42</v>
       </c>
       <c r="D20" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1218,13 +1227,13 @@
         <v>47</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>48</v>
       </c>
       <c r="D23" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="164.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1232,7 +1241,7 @@
         <v>49</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C24" t="s">
         <v>50</v>
@@ -1246,13 +1255,13 @@
         <v>51</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C25" t="s">
         <v>52</v>
       </c>
       <c r="D25" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1266,7 +1275,7 @@
         <v>54</v>
       </c>
       <c r="D26" t="s">
-        <v>35</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>